<commit_message>
committed on 12:03:2018:14:29:00PM By LOGESWARAN SUBBIAH
</commit_message>
<xml_diff>
--- a/data/Joomla url list.xlsx
+++ b/data/Joomla url list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="19820" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33420,17 +33420,141 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
     </font>
     <font>
       <b/>
@@ -33439,159 +33563,8 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -33606,187 +33579,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor indexed="42"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor indexed="44"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor indexed="29"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor indexed="26"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor indexed="55"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor indexed="47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor indexed="46"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor indexed="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor indexed="57"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor indexed="43"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor indexed="10"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor indexed="31"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor indexed="25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor indexed="49"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor indexed="27"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor indexed="53"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -33801,16 +33684,105 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="44"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="63"/>
+      </left>
+      <right style="double">
+        <color indexed="63"/>
+      </right>
+      <top style="double">
+        <color indexed="63"/>
+      </top>
+      <bottom style="double">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="63"/>
+      </left>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top style="thin">
+        <color indexed="63"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="49"/>
+      </top>
+      <bottom style="double">
+        <color indexed="49"/>
       </bottom>
       <diagonal/>
     </border>
@@ -33819,111 +33791,22 @@
       <right/>
       <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color indexed="52"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -33932,198 +33815,200 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="40% - Accent1" xfId="2"/>
+    <cellStyle name="Comma [0]" xfId="3"/>
+    <cellStyle name="Currency [0]" xfId="4"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Comma[0]" xfId="6" builtinId="6"/>
+    <cellStyle name="Percent" xfId="7" builtinId="5"/>
+    <cellStyle name="Currency[0]" xfId="8" builtinId="7"/>
+    <cellStyle name="Note" xfId="9"/>
+    <cellStyle name="Heading 2" xfId="10"/>
+    <cellStyle name="Check Cell" xfId="11"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9"/>
+    <cellStyle name="60% - Accent4" xfId="14"/>
+    <cellStyle name="Warning Text" xfId="15"/>
+    <cellStyle name="40% - Accent3" xfId="16"/>
+    <cellStyle name="Title" xfId="17"/>
+    <cellStyle name="40% - Accent2" xfId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="19"/>
+    <cellStyle name="Heading 1" xfId="20"/>
+    <cellStyle name="Heading 3" xfId="21"/>
+    <cellStyle name="Heading 4" xfId="22"/>
+    <cellStyle name="Input" xfId="23"/>
+    <cellStyle name="Output" xfId="24"/>
+    <cellStyle name="Good" xfId="25"/>
+    <cellStyle name="60% - Accent3" xfId="26"/>
+    <cellStyle name="Calculation" xfId="27"/>
+    <cellStyle name="20% - Accent1" xfId="28"/>
+    <cellStyle name="Linked Cell" xfId="29"/>
+    <cellStyle name="Total" xfId="30"/>
+    <cellStyle name="Bad" xfId="31"/>
+    <cellStyle name="Neutral" xfId="32"/>
+    <cellStyle name="Accent1" xfId="33"/>
+    <cellStyle name="60% - Accent1" xfId="34"/>
+    <cellStyle name="20% - Accent5" xfId="35"/>
+    <cellStyle name="Accent2" xfId="36"/>
+    <cellStyle name="20% - Accent2" xfId="37"/>
+    <cellStyle name="60% - Accent2" xfId="38"/>
+    <cellStyle name="20% - Accent6" xfId="39"/>
+    <cellStyle name="Accent3" xfId="40"/>
+    <cellStyle name="20% - Accent3" xfId="41"/>
+    <cellStyle name="Accent4" xfId="42"/>
+    <cellStyle name="20% - Accent4" xfId="43"/>
+    <cellStyle name="40% - Accent4" xfId="44"/>
+    <cellStyle name="Accent5" xfId="45"/>
+    <cellStyle name="40% - Accent5" xfId="46"/>
+    <cellStyle name="60% - Accent5" xfId="47"/>
+    <cellStyle name="Accent6" xfId="48"/>
+    <cellStyle name="40% - Accent6" xfId="49"/>
+    <cellStyle name="60% - Accent6" xfId="50"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -34173,71 +34058,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -34449,6 +34334,7 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -34458,7 +34344,7 @@
   <dimension ref="A1:B11114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -34966,49 +34852,65 @@
       <c r="A63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="2"/>
+      <c r="B64" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="2"/>
+      <c r="B65" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="2"/>
+      <c r="B68" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="2"/>
+      <c r="B69" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B70" s="2"/>
+      <c r="B70" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2" t="s">

</xml_diff>